<commit_message>
updating code May 21 2024
</commit_message>
<xml_diff>
--- a/inputdata/mapping.xlsx
+++ b/inputdata/mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murtuza.morbiwala.sa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murtuza.morbiwala.sa\Desktop\Python Developement\MappingAssist\inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B17E677-B838-4531-A45E-E421DFD411ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C64788-2934-490D-8335-9937589817DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D48F1668-2FE4-4BEE-A43A-0C092D0AFCAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D48F1668-2FE4-4BEE-A43A-0C092D0AFCAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="55">
   <si>
     <t>Address Line 1</t>
   </si>
@@ -192,10 +192,16 @@
     <t>TargetExplanation</t>
   </si>
   <si>
-    <t>TargetColumnType</t>
-  </si>
-  <si>
     <t>LatestAddress</t>
+  </si>
+  <si>
+    <t>InsuranceName</t>
+  </si>
+  <si>
+    <t>latestInsurance</t>
+  </si>
+  <si>
+    <t>ColumnDataType</t>
   </si>
 </sst>
 </file>
@@ -360,6 +366,104 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -425,7 +529,9 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -440,6 +546,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -448,13 +570,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -464,6 +579,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -479,122 +601,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -611,27 +617,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08E22E7F-FABC-4D53-B8EF-A462D96FE3D9}" name="SourceTable" displayName="SourceTable" ref="A1:E16" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
-  <autoFilter ref="A1:E16" xr:uid="{08E22E7F-FABC-4D53-B8EF-A462D96FE3D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08E22E7F-FABC-4D53-B8EF-A462D96FE3D9}" name="SourceTable" displayName="SourceTable" ref="A1:E17" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:E17" xr:uid="{08E22E7F-FABC-4D53-B8EF-A462D96FE3D9}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6B8CF911-B2AB-4F05-8961-578FABE854FB}" name="SourceTableName" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{7661F95C-CEDC-422C-88DD-6E1EB189D372}" name="SourceColumnName " dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{09677FB0-D29C-48E6-A4FB-5285F38F79B9}" name="SourceColumnDataType" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{B81BAB0E-865B-4A68-A55E-4F8C717588FF}" name="UniqueDataValues " dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{1E8C4A68-B8D3-448B-8C3A-592719F20365}" name="Nullable" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{6B8CF911-B2AB-4F05-8961-578FABE854FB}" name="SourceTableName" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{7661F95C-CEDC-422C-88DD-6E1EB189D372}" name="SourceColumnName " dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{09677FB0-D29C-48E6-A4FB-5285F38F79B9}" name="SourceColumnDataType" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{B81BAB0E-865B-4A68-A55E-4F8C717588FF}" name="UniqueDataValues " dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{1E8C4A68-B8D3-448B-8C3A-592719F20365}" name="Nullable" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F9FAB435-6C14-45B6-92C1-2AF45707BCB1}" name="TargetTable" displayName="TargetTable" ref="A1:D11" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:D11" xr:uid="{F9FAB435-6C14-45B6-92C1-2AF45707BCB1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F9FAB435-6C14-45B6-92C1-2AF45707BCB1}" name="TargetTable" displayName="TargetTable" ref="A1:D12" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D12" xr:uid="{F9FAB435-6C14-45B6-92C1-2AF45707BCB1}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{06A89645-FD19-441C-872C-B80134F51062}" name="TargetColumn" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{2D75AACC-EEC7-4707-872E-0D9D138BA395}" name="TargetColumnDataType" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{60CBD8CD-5CEB-4CA3-BC30-E4B8368F8766}" name="TargetExplanation" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{5F57937E-EBAB-4235-89BC-978F87089C14}" name="TargetColumnType" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{06A89645-FD19-441C-872C-B80134F51062}" name="TargetColumn" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{2D75AACC-EEC7-4707-872E-0D9D138BA395}" name="TargetColumnDataType" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{60CBD8CD-5CEB-4CA3-BC30-E4B8368F8766}" name="TargetExplanation" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{5F57937E-EBAB-4235-89BC-978F87089C14}" name="ColumnDataType" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -954,9 +960,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0C2B5C-BE01-44F2-9850-20EDE60C7C31}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1213,10 +1221,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
@@ -1229,19 +1237,36 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="C17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1255,9 +1280,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33915CE-B945-4F91-80EC-446BABABFF33}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1278,7 +1305,7 @@
         <v>50</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1314,10 +1341,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>20</v>
@@ -1328,7 +1355,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -1342,7 +1369,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -1356,7 +1383,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -1370,10 +1397,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>20</v>
@@ -1384,10 +1411,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>20</v>
@@ -1398,26 +1425,40 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a PDF and a docs folder
</commit_message>
<xml_diff>
--- a/inputdata/mapping.xlsx
+++ b/inputdata/mapping.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murtuza.morbiwala.sa\Desktop\Python Developement\MappingAssist\inputdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murtuza.morbiwala.sa\Desktop\Python Developement\Gen_AI_Mapping_Agent_Excel_Metadata\inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CD2D28-86ED-4DBC-B330-2B28D55F8038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FF3249-4A54-4832-8654-CEA8D01CA18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D48F1668-2FE4-4BEE-A43A-0C092D0AFCAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{D48F1668-2FE4-4BEE-A43A-0C092D0AFCAB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sources" sheetId="1" r:id="rId1"/>
-    <sheet name="Target" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sources1" sheetId="4" r:id="rId1"/>
+    <sheet name="Target1" sheetId="5" r:id="rId2"/>
+    <sheet name="Sources2" sheetId="1" r:id="rId3"/>
+    <sheet name="Target2" sheetId="2" r:id="rId4"/>
+    <sheet name="Queries" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="89">
   <si>
     <t>Address Line 1</t>
   </si>
@@ -187,110 +189,175 @@
     <t>InsuranceId</t>
   </si>
   <si>
-    <t>WITH patient_details AS (
-    SELECT
-        p.ID AS PATIENTID,
-        CONCAT(p.firstname, ' ', p.lastname) AS PATIENTNAME
-    FROM
-        Ptnt101 p
+    <t>TargetColumnName</t>
+  </si>
+  <si>
+    <t>TargetTableName</t>
+  </si>
+  <si>
+    <t>PatientName</t>
+  </si>
+  <si>
+    <t>PatientId</t>
+  </si>
+  <si>
+    <t>AddressLine1</t>
+  </si>
+  <si>
+    <t>TableDescription</t>
+  </si>
+  <si>
+    <t>patient table</t>
+  </si>
+  <si>
+    <t>patient insurance bridge</t>
+  </si>
+  <si>
+    <t>insurance table</t>
+  </si>
+  <si>
+    <t>address table</t>
+  </si>
+  <si>
+    <t>latest Insurance using valid from date from patient insurance bridge table</t>
+  </si>
+  <si>
+    <t>TargetColumnDataType</t>
+  </si>
+  <si>
+    <t>400050 ,  400093</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>Employee table</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Dep</t>
+  </si>
+  <si>
+    <t>EMPID</t>
+  </si>
+  <si>
+    <t>DEPID</t>
+  </si>
+  <si>
+    <t>Department Table</t>
+  </si>
+  <si>
+    <t>Employee Department table</t>
+  </si>
+  <si>
+    <t>Finance,Sales</t>
+  </si>
+  <si>
+    <t>DeptID</t>
+  </si>
+  <si>
+    <t>DeptName</t>
+  </si>
+  <si>
+    <t>DeptAddressCity</t>
+  </si>
+  <si>
+    <t>DeptAddressState</t>
+  </si>
+  <si>
+    <t>DeptAddressZip</t>
+  </si>
+  <si>
+    <t>01-10-2020,01-01-2018</t>
+  </si>
+  <si>
+    <t>Ahmedabad,Goa</t>
+  </si>
+  <si>
+    <t>Gujarat,maharastra</t>
+  </si>
+  <si>
+    <t>Latest  Address for Latest Department using valid from</t>
+  </si>
+  <si>
+    <t>Latest Department Name using valid from</t>
+  </si>
+  <si>
+    <t>Latest Department ID using valid from</t>
+  </si>
+  <si>
+    <t>01-10-2000,01-01-2005</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>EmployeeID</t>
+  </si>
+  <si>
+    <t>EmployeeName</t>
+  </si>
+  <si>
+    <t>WITH LatestInsurance AS (
+  SELECT ptnt.ID AS PatientID,
+         ptins.insid AS InsuranceID,
+         ins.name AS InsuranceName,
+         ROW_NUMBER() OVER (PARTITION BY ptnt.ID ORDER BY ptins.ValidFrom DESC) AS rn
+  FROM Ptnt101 ptnt
+  LEFT JOIN PTINS101 ptins ON ptnt.ID = ptins.ptntid
+  LEFT JOIN INS101 ins ON ptins.insid = ins.Id
 ),
-latest_insurance AS (
-    SELECT
-        pd.PATIENTID,
-        pt.insid,
-        i.name AS InsuranceName,
-        ROW_NUMBER() OVER (PARTITION BY pd.PATIENTID ORDER BY pt.ValidFrom DESC) AS row_num
-    FROM
-        patient_details pd
-        INNER JOIN PTINS101 pt ON pd.PATIENTID = pt.ptntid
-        INNER JOIN INS101 i ON pt.insid = i.Id
+LatestInsuranceAddress AS (
+  SELECT li.PatientID,
+         li.InsuranceID,
+         li.InsuranceName,
+         a.ID AS AddressId,
+         a."Address Line 1" AS InsuranceAddressLine1,
+         a.City AS InsuranceCity,
+         a.State AS InsuranceState,
+         a.Zip AS InsuranceZip,
+         ROW_NUMBER() OVER (PARTITION BY li.PatientID, li.InsuranceID ORDER BY a.ValidFrom DESC) AS rn
+  FROM LatestInsurance li
+  LEFT JOIN ADD101 a ON li.InsuranceID = a.INSID
 ),
-insurance_address AS (
-    SELECT
-        li.PATIENTID,
-        li.insid,
-        li.InsuranceName,
-        a."Address Line 1" AS InsuranceAddressLine1,
-        a.City AS InsuranceCity,
-        a.State AS InsuranceState,
-        a.Zip AS InsuranceZip,
-        ROW_NUMBER() OVER (PARTITION BY li.PATIENTID, li.insid ORDER BY a.ValidFrom DESC) AS row_num
-    FROM
-        latest_insurance li
-        INNER JOIN ADD101 a ON a.ptntid = li.PATIENTID AND a.INSID = li.insid AND a.AddType = 'I'
-    WHERE
-        li.row_num = 1
+LatestAddress AS (
+  SELECT ptnt.ID AS PatientID,
+         a.ID AS AddressId,
+         a."Address Line 1" AS AddressLine1,
+         a.City AS City,
+         a.State AS State,
+         a.Zip AS Zip,
+         ROW_NUMBER() OVER (PARTITION BY ptnt.ID ORDER BY a.ValidFrom DESC) AS rn
+  FROM Ptnt101 ptnt
+  LEFT JOIN ADD101 a ON ptnt.ID = a.ptntid
+  WHERE a.AddType = 'H'
 ),
-home_address AS (
-    SELECT
-        pd.PATIENTID,
-        "Address Line 1",
-        City,
-        State,
-        Zip,
-        ROW_NUMBER() OVER (PARTITION BY pd.PATIENTID ORDER BY ValidFrom DESC) AS row_num
-    FROM
-        patient_details pd
-        INNER JOIN ADD101 ON ADD101.ptntid = pd.PATIENTID
-    WHERE
-        AddType = 'H'
-)
-SELECT
-    pd.PATIENTID,
-    pd.PATIENTNAME,
-    ia.InsuranceName,
-    ia.insid AS InsuranceId,
-    ia.InsuranceAddressLine1,
-    ia.InsuranceCity,
-    ia.InsuranceState,
-    ia.InsuranceZip,
-    ha."Address Line 1",
-    ha.City,
-    ha.State,
-    ha.Zip
-FROM
-    patient_details pd
-    LEFT JOIN insurance_address ia ON pd.PATIENTID = ia.PATIENTID AND ia.row_num = 1
-    LEFT JOIN home_address ha ON pd.PATIENTID = ha.PATIENTID AND ha.row_num = 1</t>
-  </si>
-  <si>
-    <t>TargetColumnName</t>
-  </si>
-  <si>
-    <t>TargetTableName</t>
-  </si>
-  <si>
-    <t>PatientName</t>
-  </si>
-  <si>
-    <t>PatientId</t>
-  </si>
-  <si>
-    <t>AddressLine1</t>
-  </si>
-  <si>
-    <t>TableDescription</t>
-  </si>
-  <si>
-    <t>patient table</t>
-  </si>
-  <si>
-    <t>patient insurance bridge</t>
-  </si>
-  <si>
-    <t>insurance table</t>
-  </si>
-  <si>
-    <t>address table</t>
-  </si>
-  <si>
-    <t>latest Insurance using valid from date from patient insurance bridge table</t>
-  </si>
-  <si>
-    <t>TargetColumnDataType</t>
-  </si>
-  <si>
-    <t>400050 ,  400093</t>
+-- Final Query
+SELECT ptnt.ID AS PatientId,
+       CONCAT(CAST(ptnt.firstname AS VARCHAR(100)), ' ', CAST(ptnt.lastname AS VARCHAR(100))) AS PatientName,
+       lia.InsuranceName,
+       CAST(lia.InsuranceID AS VARCHAR(20)) AS InsuranceId,
+       lia.InsuranceAddressLine1,
+       lia.InsuranceCity,
+       lia.InsuranceState,
+       lia.InsuranceZip,
+       la.AddressLine1,
+       la.City,
+       la.State,
+       la.Zip
+FROM Ptnt101 ptnt
+LEFT JOIN LatestInsurance lia ON ptnt.ID = lia.PatientID
+LEFT JOIN LatestInsuranceAddress lia ON lia.PatientID = lia.PatientID AND lia.InsuranceID = lia.InsuranceID
+LEFT JOIN LatestAddress la ON ptnt.ID = la.PatientID
+WHERE lia.rn = 1 AND la.rn = 1;</t>
+  </si>
+  <si>
+    <t>Query  Example</t>
   </si>
 </sst>
 </file>
@@ -456,7 +523,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="36">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -696,6 +763,260 @@
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
@@ -725,6 +1046,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1D66BABB-62F2-4F79-977D-D99F8E5243EC}" name="SourceTable3" displayName="SourceTable3" ref="A1:F14" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+  <autoFilter ref="A1:F14" xr:uid="{08E22E7F-FABC-4D53-B8EF-A462D96FE3D9}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{F054841D-7585-4CCC-93B7-CF8A5DC49DAF}" name="SourceTableName" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{C37601F3-6116-4FAB-93AA-9F106F6D8375}" name="SourceColumnName " dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{3B667EC6-A349-4C96-81AF-5E19125895B7}" name="SourceColumnDataType" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{62981453-CABD-4CBF-A4E3-176FE1884334}" name="UniqueDataValues " dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{216683B9-834A-4899-82DB-A4DCC1479274}" name="TableDescription" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{536ED885-F804-47F3-802C-070704D00244}" name="Nullable" dataDxfId="26"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F43934E6-B695-4413-9AB9-AD2B6D2D2EB3}" name="TargetTable5" displayName="TargetTable5" ref="A1:D8" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="A1:D8" xr:uid="{F9FAB435-6C14-45B6-92C1-2AF45707BCB1}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{927B7884-2CED-4438-B4A2-737B25884CA3}" name="TargetTableName" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{575F0501-155E-4371-8D1D-7B03F8094D1A}" name="TargetColumnName" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{E8CDBB73-5439-4715-A47F-F032CB9C6A96}" name="TargetExplanation" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{91A090C8-EFDB-42BC-A9A4-828ACC75595C}" name="TargetColumnDataType" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08E22E7F-FABC-4D53-B8EF-A462D96FE3D9}" name="SourceTable" displayName="SourceTable" ref="A1:F18" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A1:F18" xr:uid="{08E22E7F-FABC-4D53-B8EF-A462D96FE3D9}"/>
   <tableColumns count="6">
@@ -739,7 +1088,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F9FAB435-6C14-45B6-92C1-2AF45707BCB1}" name="TargetTable" displayName="TargetTable" ref="A1:D13" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A1:D13" xr:uid="{F9FAB435-6C14-45B6-92C1-2AF45707BCB1}"/>
   <tableColumns count="4">
@@ -1068,11 +1417,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0C2B5C-BE01-44F2-9850-20EDE60C7C31}">
-  <dimension ref="A1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2C335C-8C2C-4895-B1F8-0480C1A8E963}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,7 +1454,7 @@
         <v>42</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>43</v>
@@ -1113,7 +1462,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -1125,7 +1474,7 @@
         <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>23</v>
@@ -1133,7 +1482,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -1145,7 +1494,7 @@
         <v>27</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>24</v>
@@ -1153,7 +1502,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -1165,7 +1514,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>24</v>
@@ -1173,10 +1522,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -1185,7 +1534,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>23</v>
@@ -1193,19 +1542,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>23</v>
@@ -1213,19 +1562,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>23</v>
@@ -1233,10 +1582,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
@@ -1245,7 +1594,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>23</v>
@@ -1253,19 +1602,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>24</v>
@@ -1273,7 +1622,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -1282,10 +1631,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>24</v>
@@ -1293,7 +1642,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>2</v>
@@ -1302,10 +1651,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>24</v>
@@ -1313,7 +1662,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -1322,10 +1671,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>24</v>
@@ -1333,7 +1682,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>
@@ -1342,10 +1691,10 @@
         <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>23</v>
@@ -1353,101 +1702,21 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1460,11 +1729,539 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF79EE5C-23A2-4C82-8B76-DC56E4D1A7A4}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0C2B5C-BE01-44F2-9850-20EDE60C7C31}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="A1:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33915CE-B945-4F91-80EC-446BABABFF33}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,16 +2274,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1494,7 +2291,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -1508,7 +2305,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>17</v>
@@ -1525,7 +2322,7 @@
         <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>18</v>
@@ -1539,7 +2336,7 @@
         <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>18</v>
@@ -1606,7 +2403,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>46</v>
@@ -1665,12 +2462,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A66F24D-9E0A-475A-8E30-7015ADF18BC9}">
-  <dimension ref="C4"/>
+  <dimension ref="C4:C5"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1678,9 +2475,14 @@
     <col min="3" max="3" width="128" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C4" s="11" t="s">
-        <v>49</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="C5" s="11" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>